<commit_message>
commit main test suite
</commit_message>
<xml_diff>
--- a/Data Files/Users.xlsx
+++ b/Data Files/Users.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekapangaribuan/Desktop/Automation-Project/katalon-api-placeholder/Data Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C335B26-5A52-C64B-9E6A-91CDBBCB723B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DC24FB-561F-FE48-A848-E1B66E111326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15300" xr2:uid="{92583B61-D12B-5D43-AC6A-D9AE4FDAB631}"/>
   </bookViews>
   <sheets>
     <sheet name="Get-Users" sheetId="1" r:id="rId1"/>
+    <sheet name="Add-Users" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -50,9 +51,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>street</t>
   </si>
   <si>
@@ -65,9 +63,6 @@
     <t>zipcode</t>
   </si>
   <si>
-    <t>geo</t>
-  </si>
-  <si>
     <t>lat</t>
   </si>
   <si>
@@ -80,9 +75,6 @@
     <t>website</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>catchPhrase</t>
   </si>
   <si>
@@ -117,13 +109,130 @@
   </si>
   <si>
     <t>anastasia.net</t>
+  </si>
+  <si>
+    <t>Cristiano Ronaldo</t>
+  </si>
+  <si>
+    <t>Cr7</t>
+  </si>
+  <si>
+    <t>Lionel Messi</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>cr7@april.biz</t>
+  </si>
+  <si>
+    <t>messi@melissa.tv</t>
+  </si>
+  <si>
+    <t>Buenos Street 01</t>
+  </si>
+  <si>
+    <t>Apt. 001</t>
+  </si>
+  <si>
+    <t>Paolo 001</t>
+  </si>
+  <si>
+    <t>Buenos Street 02</t>
+  </si>
+  <si>
+    <t>Apt. 002</t>
+  </si>
+  <si>
+    <t>Paolo 002</t>
+  </si>
+  <si>
+    <t>cr7.org</t>
+  </si>
+  <si>
+    <t>lm.org</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>cr7 corp</t>
+  </si>
+  <si>
+    <t>lm corp</t>
+  </si>
+  <si>
+    <t>best player</t>
+  </si>
+  <si>
+    <t>best player 001</t>
+  </si>
+  <si>
+    <t>best match</t>
+  </si>
+  <si>
+    <t>best match 001</t>
+  </si>
+  <si>
+    <t>Kulas Light</t>
+  </si>
+  <si>
+    <t>Apt. 556</t>
+  </si>
+  <si>
+    <t>Gwenborough</t>
+  </si>
+  <si>
+    <t>92998-3874</t>
+  </si>
+  <si>
+    <t>Romaguera-Crona</t>
+  </si>
+  <si>
+    <t>Multi-layered client-server neural-net</t>
+  </si>
+  <si>
+    <t>harness real-time e-markets</t>
+  </si>
+  <si>
+    <t>synergize scalable supply-chains</t>
+  </si>
+  <si>
+    <t>Proactive didactic contingency</t>
+  </si>
+  <si>
+    <t>Deckow-Crist</t>
+  </si>
+  <si>
+    <t>90566-7771</t>
+  </si>
+  <si>
+    <t>Wisokyburgh</t>
+  </si>
+  <si>
+    <t>Suite 879</t>
+  </si>
+  <si>
+    <t>Victor Plains</t>
+  </si>
+  <si>
+    <t>-37.3159</t>
+  </si>
+  <si>
+    <t>-43.9509</t>
+  </si>
+  <si>
+    <t>81.1496</t>
+  </si>
+  <si>
+    <t>-34.4618</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +250,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -167,10 +282,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,20 +602,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051AD4AB-8622-9447-BA87-D7A3362A8F74}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,19 +634,19 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
@@ -537,62 +656,107 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="N2" t="s">
-        <v>21</v>
+        <v>50</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -601,5 +765,168 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{C1DE5410-31E1-F042-833C-6FEE8BEDB6DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="I2:I3 J2:J3" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD0B121-2CDB-0445-8A68-A61D02C41602}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>1232575</v>
+      </c>
+      <c r="H2">
+        <v>-390192</v>
+      </c>
+      <c r="I2">
+        <v>109780</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>7047346</v>
+      </c>
+      <c r="H3">
+        <v>-390194</v>
+      </c>
+      <c r="I3">
+        <v>109710</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="Sincere@april.biz" xr:uid="{321683AC-EEC7-D24B-9F9B-2CBA408FB112}"/>
+    <hyperlink ref="C3" r:id="rId2" display="Shanna@melissa.tv" xr:uid="{4BCD1F9A-326D-EF4A-A99B-F167A9F70FB5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>